<commit_message>
motor dizayn edildi ama verim çok düşük çıkıyor
küçük boyutlu motorda verimi artırmak biraz daha zor oluyor gibi
</commit_message>
<xml_diff>
--- a/design_parameter.xlsx
+++ b/design_parameter.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>N</t>
   </si>
@@ -186,9 +186,6 @@
     <t>B,ml,max</t>
   </si>
   <si>
-    <t>Is,Iph</t>
-  </si>
-  <si>
     <t>A/m</t>
   </si>
   <si>
@@ -210,7 +207,16 @@
     <t>output power</t>
   </si>
   <si>
-    <t>input power</t>
+    <t>eff</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>pf</t>
+  </si>
+  <si>
+    <t>Is</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,10 +645,10 @@
     <col min="8" max="8" width="11.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="6"/>
     <col min="10" max="10" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="24" style="6" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="6"/>
     <col min="13" max="13" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="6"/>
+    <col min="14" max="14" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" style="6" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -669,13 +675,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="7">
-        <f>E6/4.44/B3/E14/B45/K13</f>
-        <v>782.06580042199994</v>
+        <f>K5*B39</f>
+        <v>840</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="6">
         <f>E6/4.44/B3/K13/E14/B45</f>
-        <v>782.06580042199994</v>
+        <v>854.40726984983814</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -718,17 +724,16 @@
         <v>0</v>
       </c>
       <c r="K5" s="9">
-        <f>K3/B39</f>
-        <v>65.172150035166666</v>
+        <v>70</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="6">
         <f>M3/B39</f>
-        <v>65.172150035166666</v>
+        <v>71.200605820819845</v>
       </c>
       <c r="O5" s="6">
         <f>K13*B8*0.001/K11/9/4/3.14/0.0000001</f>
-        <v>11.282870395043656</v>
+        <v>32.9</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -736,8 +741,8 @@
         <v>26</v>
       </c>
       <c r="E6" s="7">
-        <f>E4-10</f>
-        <v>371.05117766515298</v>
+        <f>E4</f>
+        <v>381.05117766515298</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>27</v>
@@ -750,7 +755,7 @@
       </c>
       <c r="K6" s="7">
         <f>B38*K5</f>
-        <v>586.54935031649995</v>
+        <v>630</v>
       </c>
       <c r="L6" s="4"/>
     </row>
@@ -812,14 +817,15 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3">
-        <v>30000</v>
+      <c r="K10" s="2">
+        <f>K5*B36*B31*K11/3.14/B12*1000</f>
+        <v>10282.140885686482</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -831,13 +837,17 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="K11" s="7">
-        <f>K10*3.14*B15*0.001/(B36*K5*B31)</f>
-        <v>1.0929336467983961</v>
+        <f>B8*0.001/K6/4/3.14/0.0000001</f>
+        <v>0.35232653392024915</v>
       </c>
       <c r="L11" s="4"/>
+      <c r="M11" s="6">
+        <f>B8*0.001/K6/4/3.14/0.0000001</f>
+        <v>0.35232653392024915</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
@@ -853,7 +863,7 @@
       </c>
       <c r="H12" s="2">
         <f>E6*B8*(0.001)/(4.44*B3*B38*B39*K5*K5*E14*4*3.14*(0.0000001)*B45)</f>
-        <v>0.1892131636067664</v>
+        <v>0.16843364930113633</v>
       </c>
       <c r="I12" s="4"/>
       <c r="L12" s="4"/>
@@ -883,12 +893,12 @@
         <v>15</v>
       </c>
       <c r="K13" s="3">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="6">
         <f>E16/E14</f>
-        <v>1.2672224534564301E-4</v>
+        <v>1.2116198001727557E-4</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -916,7 +926,7 @@
       </c>
       <c r="K14" s="7">
         <f>K13*3.14/2</f>
-        <v>0.78500000000000003</v>
+        <v>0.7379</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -939,7 +949,7 @@
       </c>
       <c r="K15" s="2">
         <f>K14*B25*0.9</f>
-        <v>2.0111818912095476</v>
+        <v>1.8905109777369749</v>
       </c>
       <c r="L15" s="4"/>
     </row>
@@ -949,7 +959,7 @@
       </c>
       <c r="E16" s="2">
         <f>K6*H12*E14*4*3.14*0.0000001/(B17*0.01)</f>
-        <v>6.0183562370779518E-7</v>
+        <v>5.7542853359704609E-7</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -961,7 +971,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:14">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -974,7 +984,7 @@
       <c r="I17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:14">
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -984,13 +994,13 @@
       </c>
       <c r="K18" s="4">
         <f>K10*K13</f>
-        <v>15000</v>
+        <v>4832.6062162726466</v>
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1">
+    <row r="19" spans="1:14" ht="18" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1">
         <v>4.47</v>
@@ -1004,13 +1014,13 @@
       </c>
       <c r="K19" s="4">
         <f>K18*B15*B15/4*110*2*3.14*0.000000001</f>
-        <v>7.6781832638952716</v>
+        <v>2.4737090780520594</v>
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1">
         <v>12</v>
@@ -1019,18 +1029,11 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K20" s="6">
-        <f>1500/60*2*3.14*K19</f>
-        <v>1205.4747724315575</v>
-      </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2">
         <f>(3.14*(B12+2*B20)-B31*B19)/B31</f>
@@ -1040,14 +1043,11 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:14">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2">
         <f>B19+B21</f>
@@ -1057,9 +1057,21 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
+      <c r="J22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" s="1">
+        <v>80</v>
+      </c>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1068,20 +1080,25 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:14">
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" s="2">
+        <f>11*K13*K10*B45*K22*N22*0.001</f>
+        <v>3444.6817109591425</v>
+      </c>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="45">
+    <row r="25" spans="1:14" ht="45">
       <c r="A25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1">
         <f>B22/B21</f>
@@ -1091,13 +1108,21 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4">
+        <f>K10*K13*B12*B12/2*3.14*B17*0.000000001</f>
+        <v>2.5246380579896153</v>
+      </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K25" s="2">
+        <f>K24*B12*B12*B17*B5/60*2*3.14*0.000000001</f>
+        <v>179.9562007734998</v>
+      </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:14">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1108,7 +1133,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:14">
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1121,7 +1146,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:14">
       <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
@@ -1141,7 +1166,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:14">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1157,7 +1182,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:14">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1171,7 +1196,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:14">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1214,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:14">
       <c r="A32" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>